<commit_message>
data: add batch 2 customer locations (HICOOL, Drive&Control, Essar, Parkash, N-Rack, Uddishtaa)
</commit_message>
<xml_diff>
--- a/data/masters/customer_master.xlsx
+++ b/data/masters/customer_master.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C273"/>
+  <dimension ref="A1:C277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5074,6 +5074,74 @@
         </is>
       </c>
     </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>HICOOL ELECTRONIC INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>MUMBAI</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>MAHARASHTRA</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>HCE DYNAMICS PRIVATE LIMITED</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>MUMBAI</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>MAHARASHTRA</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>PARKASH ELECTRIC COMPANY</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>CHANDIGARH</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>CHANDIGARH</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>N-RACK ACCESSORIES PVT LTD</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>BANGALORE</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>KARNATAKA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data: merge Palghar, Vasai, Navi Mumbai into Mumbai
</commit_message>
<xml_diff>
--- a/data/masters/customer_master.xlsx
+++ b/data/masters/customer_master.xlsx
@@ -883,7 +883,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>NEW MUMBAI</t>
+          <t>MUMBAI</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>VASAI</t>
+          <t>MUMBAI</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>PALGHAR</t>
+          <t>MUMBAI</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3484,7 +3484,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>VASAI</t>
+          <t>MUMBAI</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -3807,7 +3807,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>VASAI</t>
+          <t>MUMBAI</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>NEW MUMBAI</t>
+          <t>MUMBAI</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -4283,7 +4283,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>NEW MUMBAI</t>
+          <t>MUMBAI</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>VASAI</t>
+          <t>MUMBAI</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -4844,7 +4844,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>VASAI</t>
+          <t>MUMBAI</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">

</xml_diff>